<commit_message>
Added time complexity reports
</commit_message>
<xml_diff>
--- a/Отчёт/First - first version.xlsx
+++ b/Отчёт/First - first version.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ислам\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Construction and analysis of algorithms\SortAlgorithms\Отчёт\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{89DEBEC0-AADE-4FC6-86FC-4031A6C42377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7934821A-A612-4BCF-9405-56C69977F0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -70,19 +67,19 @@
     <t>From 0 to 5</t>
   </si>
   <si>
-    <t>From 1 to 4100</t>
-  </si>
-  <si>
     <t>Almost Sorted</t>
   </si>
   <si>
     <t>Reversed sorted</t>
   </si>
+  <si>
+    <t>From 0 to 4000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2214,7 +2211,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2635,19 +2631,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>From </a:t>
+              <a:t>From 0 to </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="ru-RU"/>
-              <a:t>1</a:t>
+              <a:t>4</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t> to </a:t>
+              <a:t>0</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="ru-RU"/>
-              <a:t>4100</a:t>
+              <a:t>00</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -10880,322 +10876,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Задание 1"/>
-      <sheetName val="Задание 2"/>
-      <sheetName val="Задание 3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="D1">
-            <v>1970</v>
-          </cell>
-          <cell r="E1">
-            <v>1971</v>
-          </cell>
-          <cell r="F1">
-            <v>1972</v>
-          </cell>
-          <cell r="G1">
-            <v>1973</v>
-          </cell>
-          <cell r="H1">
-            <v>1974</v>
-          </cell>
-          <cell r="I1">
-            <v>1975</v>
-          </cell>
-          <cell r="J1">
-            <v>1976</v>
-          </cell>
-          <cell r="K1">
-            <v>1977</v>
-          </cell>
-          <cell r="L1">
-            <v>1978</v>
-          </cell>
-          <cell r="M1">
-            <v>1979</v>
-          </cell>
-          <cell r="N1">
-            <v>1980</v>
-          </cell>
-          <cell r="O1">
-            <v>1981</v>
-          </cell>
-          <cell r="P1">
-            <v>1982</v>
-          </cell>
-          <cell r="Q1">
-            <v>1983</v>
-          </cell>
-          <cell r="R1">
-            <v>1984</v>
-          </cell>
-          <cell r="S1">
-            <v>1985</v>
-          </cell>
-          <cell r="T1">
-            <v>1986</v>
-          </cell>
-          <cell r="U1">
-            <v>1987</v>
-          </cell>
-          <cell r="V1">
-            <v>1988</v>
-          </cell>
-          <cell r="W1">
-            <v>1989</v>
-          </cell>
-          <cell r="X1">
-            <v>1990</v>
-          </cell>
-          <cell r="Y1">
-            <v>1991</v>
-          </cell>
-          <cell r="Z1">
-            <v>1992</v>
-          </cell>
-          <cell r="AA1">
-            <v>1993</v>
-          </cell>
-          <cell r="AB1">
-            <v>1994</v>
-          </cell>
-          <cell r="AC1">
-            <v>1995</v>
-          </cell>
-          <cell r="AD1">
-            <v>1996</v>
-          </cell>
-          <cell r="AE1">
-            <v>1997</v>
-          </cell>
-          <cell r="AF1">
-            <v>1998</v>
-          </cell>
-          <cell r="AG1">
-            <v>1999</v>
-          </cell>
-          <cell r="AH1">
-            <v>2000</v>
-          </cell>
-          <cell r="AI1">
-            <v>2001</v>
-          </cell>
-          <cell r="AJ1">
-            <v>2002</v>
-          </cell>
-          <cell r="AK1">
-            <v>2003</v>
-          </cell>
-          <cell r="AL1">
-            <v>2004</v>
-          </cell>
-          <cell r="AM1">
-            <v>2005</v>
-          </cell>
-          <cell r="AN1">
-            <v>2006</v>
-          </cell>
-          <cell r="AO1">
-            <v>2007</v>
-          </cell>
-          <cell r="AP1">
-            <v>2008</v>
-          </cell>
-          <cell r="AQ1">
-            <v>2009</v>
-          </cell>
-          <cell r="AR1">
-            <v>2010</v>
-          </cell>
-          <cell r="AS1">
-            <v>2011</v>
-          </cell>
-          <cell r="AT1">
-            <v>2012</v>
-          </cell>
-          <cell r="AU1">
-            <v>2013</v>
-          </cell>
-          <cell r="AV1">
-            <v>2014</v>
-          </cell>
-          <cell r="AW1">
-            <v>2015</v>
-          </cell>
-          <cell r="AX1">
-            <v>2016</v>
-          </cell>
-          <cell r="AY1">
-            <v>2017</v>
-          </cell>
-          <cell r="AZ1">
-            <v>2018</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="D2">
-            <v>24874300173831.699</v>
-          </cell>
-          <cell r="E2">
-            <v>26292119869909.531</v>
-          </cell>
-          <cell r="F2">
-            <v>28053676403134.602</v>
-          </cell>
-          <cell r="G2">
-            <v>30157706344799.457</v>
-          </cell>
-          <cell r="H2">
-            <v>32721118964678.871</v>
-          </cell>
-          <cell r="I2">
-            <v>35077076590711.34</v>
-          </cell>
-          <cell r="J2">
-            <v>37621200865650.367</v>
-          </cell>
-          <cell r="K2">
-            <v>41734672053042.203</v>
-          </cell>
-          <cell r="L2">
-            <v>46471603193524.188</v>
-          </cell>
-          <cell r="M2">
-            <v>51749366049596.359</v>
-          </cell>
-          <cell r="N2">
-            <v>57670129889441.375</v>
-          </cell>
-          <cell r="O2">
-            <v>62696470432628.516</v>
-          </cell>
-          <cell r="P2">
-            <v>62079832994561.289</v>
-          </cell>
-          <cell r="Q2">
-            <v>60217454850440.117</v>
-          </cell>
-          <cell r="R2">
-            <v>62068546364770.18</v>
-          </cell>
-          <cell r="S2">
-            <v>64532400802462.977</v>
-          </cell>
-          <cell r="T2">
-            <v>64537875660197.328</v>
-          </cell>
-          <cell r="U2">
-            <v>67330811162024.352</v>
-          </cell>
-          <cell r="V2">
-            <v>71611728767511.672</v>
-          </cell>
-          <cell r="W2">
-            <v>75763608187626.125</v>
-          </cell>
-          <cell r="X2">
-            <v>78106594612256.516</v>
-          </cell>
-          <cell r="Y2">
-            <v>80034671049190.984</v>
-          </cell>
-          <cell r="Z2">
-            <v>81475316690593.313</v>
-          </cell>
-          <cell r="AA2">
-            <v>84849934769567.969</v>
-          </cell>
-          <cell r="AB2">
-            <v>87475339624718.391</v>
-          </cell>
-          <cell r="AC2">
-            <v>92232526614369.266</v>
-          </cell>
-          <cell r="AD2">
-            <v>92616277442463.469</v>
-          </cell>
-          <cell r="AE2">
-            <v>95381929962177.156</v>
-          </cell>
-          <cell r="AF2">
-            <v>95944323417142.234</v>
-          </cell>
-          <cell r="AG2">
-            <v>94508566008583.031</v>
-          </cell>
-          <cell r="AH2">
-            <v>91365779054363.25</v>
-          </cell>
-          <cell r="AI2">
-            <v>93239151351215.969</v>
-          </cell>
-          <cell r="AJ2">
-            <v>107251654045629.92</v>
-          </cell>
-          <cell r="AK2">
-            <v>111885723183397.83</v>
-          </cell>
-          <cell r="AL2">
-            <v>116425396233849.05</v>
-          </cell>
-          <cell r="AM2">
-            <v>118909323321177.66</v>
-          </cell>
-          <cell r="AN2">
-            <v>124625433843091.53</v>
-          </cell>
-          <cell r="AO2">
-            <v>131382154852485.27</v>
-          </cell>
-          <cell r="AP2">
-            <v>139736904780325.02</v>
-          </cell>
-          <cell r="AQ2">
-            <v>139376423483631.27</v>
-          </cell>
-          <cell r="AR2">
-            <v>154908163875603.94</v>
-          </cell>
-          <cell r="AS2">
-            <v>161490383775856.41</v>
-          </cell>
-          <cell r="AT2">
-            <v>160620737158288.97</v>
-          </cell>
-          <cell r="AU2">
-            <v>174140980134935</v>
-          </cell>
-          <cell r="AV2">
-            <v>182605782269406.16</v>
-          </cell>
-          <cell r="AW2">
-            <v>188230723323461</v>
-          </cell>
-          <cell r="AX2">
-            <v>196348935544778.66</v>
-          </cell>
-          <cell r="AY2">
-            <v>206075614589314.06</v>
-          </cell>
-          <cell r="AZ2">
-            <v>212991866469856</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -11492,11 +11172,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AO31" sqref="AO31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AN60" sqref="AN60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12647,7 +12327,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B27">
         <v>50</v>
@@ -12691,7 +12371,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B28">
         <v>60</v>
@@ -12735,7 +12415,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B29">
         <v>70</v>
@@ -12779,7 +12459,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B30">
         <v>80</v>
@@ -12823,7 +12503,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B31">
         <v>90</v>
@@ -12867,7 +12547,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B32">
         <v>100</v>
@@ -12911,7 +12591,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B33">
         <v>110</v>
@@ -12955,7 +12635,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B34">
         <v>120</v>
@@ -12999,7 +12679,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B35">
         <v>130</v>
@@ -13043,7 +12723,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B36">
         <v>140</v>
@@ -13087,7 +12767,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B37">
         <v>150</v>
@@ -13131,7 +12811,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B38">
         <v>160</v>
@@ -13175,7 +12855,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B39">
         <v>170</v>
@@ -13219,7 +12899,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B40">
         <v>180</v>
@@ -13263,7 +12943,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B41">
         <v>190</v>
@@ -13307,7 +12987,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B42">
         <v>200</v>
@@ -13351,7 +13031,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B43">
         <v>210</v>
@@ -13395,7 +13075,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B44">
         <v>220</v>
@@ -13439,7 +13119,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B45">
         <v>230</v>
@@ -13483,7 +13163,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B46">
         <v>240</v>
@@ -13527,7 +13207,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B47">
         <v>250</v>
@@ -13571,7 +13251,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B48">
         <v>260</v>
@@ -13615,7 +13295,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B49">
         <v>270</v>
@@ -13659,7 +13339,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B50">
         <v>280</v>
@@ -13703,7 +13383,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B51">
         <v>290</v>
@@ -13747,7 +13427,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B52">
         <v>50</v>
@@ -13791,7 +13471,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B53">
         <v>60</v>
@@ -13835,7 +13515,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B54">
         <v>70</v>
@@ -13879,7 +13559,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B55">
         <v>80</v>
@@ -13923,7 +13603,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B56">
         <v>90</v>
@@ -13967,7 +13647,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B57">
         <v>100</v>
@@ -14011,7 +13691,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B58">
         <v>110</v>
@@ -14055,7 +13735,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B59">
         <v>120</v>
@@ -14099,7 +13779,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B60">
         <v>130</v>
@@ -14143,7 +13823,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B61">
         <v>140</v>
@@ -14187,7 +13867,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B62">
         <v>150</v>
@@ -14231,7 +13911,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B63">
         <v>160</v>
@@ -14275,7 +13955,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B64">
         <v>170</v>
@@ -14319,7 +13999,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B65">
         <v>180</v>
@@ -14363,7 +14043,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B66">
         <v>190</v>
@@ -14407,7 +14087,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B67">
         <v>200</v>
@@ -14451,7 +14131,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B68">
         <v>210</v>
@@ -14495,7 +14175,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B69">
         <v>220</v>
@@ -14539,7 +14219,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B70">
         <v>230</v>
@@ -14583,7 +14263,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B71">
         <v>240</v>
@@ -14627,7 +14307,7 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B72">
         <v>250</v>
@@ -14671,7 +14351,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B73">
         <v>260</v>
@@ -14715,7 +14395,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B74">
         <v>270</v>
@@ -14759,7 +14439,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B75">
         <v>280</v>
@@ -14803,7 +14483,7 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B76">
         <v>290</v>
@@ -14847,7 +14527,7 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B77">
         <v>50</v>
@@ -14891,7 +14571,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B78">
         <v>60</v>
@@ -14935,7 +14615,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B79">
         <v>70</v>
@@ -14979,7 +14659,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B80">
         <v>80</v>
@@ -15023,7 +14703,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B81">
         <v>90</v>
@@ -15067,7 +14747,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B82">
         <v>100</v>
@@ -15111,7 +14791,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B83">
         <v>110</v>
@@ -15155,7 +14835,7 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B84">
         <v>120</v>
@@ -15199,7 +14879,7 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B85">
         <v>130</v>
@@ -15243,7 +14923,7 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B86">
         <v>140</v>
@@ -15287,7 +14967,7 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B87">
         <v>150</v>
@@ -15331,7 +15011,7 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B88">
         <v>160</v>
@@ -15375,7 +15055,7 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B89">
         <v>170</v>
@@ -15419,7 +15099,7 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B90">
         <v>180</v>
@@ -15463,7 +15143,7 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B91">
         <v>190</v>
@@ -15507,7 +15187,7 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B92">
         <v>200</v>
@@ -15551,7 +15231,7 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B93">
         <v>210</v>
@@ -15595,7 +15275,7 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B94">
         <v>220</v>
@@ -15639,7 +15319,7 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B95">
         <v>230</v>
@@ -15683,7 +15363,7 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B96">
         <v>240</v>
@@ -15727,7 +15407,7 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B97">
         <v>250</v>
@@ -15771,7 +15451,7 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B98">
         <v>260</v>
@@ -15815,7 +15495,7 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B99">
         <v>270</v>
@@ -15859,7 +15539,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B100">
         <v>280</v>
@@ -15903,7 +15583,7 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B101">
         <v>290</v>

</xml_diff>